<commit_message>
Changes to be committed: 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2020 Datasheets & Spreadsheets_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2022 Datasheets & Spreadsheets_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2023 Datasheets & Spreadsheets_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2024 Datasheets & Spreadsheets_combined.xlsx
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform - Color-wise graphs/2023 Datasheets & Spreadsheets_combined.xlsx
+++ b/Extracted Data/VRU Headform - Color-wise graphs/2023 Datasheets & Spreadsheets_combined.xlsx
@@ -443,12 +443,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Input Sheet</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
@@ -474,12 +474,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Input Sheet</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
@@ -505,12 +505,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Input Sheet</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
@@ -536,12 +536,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Input Sheet</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
@@ -567,12 +567,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Input Sheet</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
@@ -598,12 +598,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Input Sheet</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
@@ -629,12 +629,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Input Sheet</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
@@ -660,12 +660,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Input Sheet</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>

</xml_diff>